<commit_message>
dicsounted rate is added
</commit_message>
<xml_diff>
--- a/data/LCOE_Parameters.xlsx
+++ b/data/LCOE_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanko\Desktop\personal\coding\OPV_SBSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245F0FEF-2D89-4289-A377-19EB4BD2A40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF71121-27C4-4916-ACD1-3132EF372AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="131">
   <si>
     <t>LCOE</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>MW</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Y0</t>
@@ -629,6 +626,12 @@
   </si>
   <si>
     <t>£/panel</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Yearly (to be in all arrays needed ;*)</t>
   </si>
 </sst>
 </file>
@@ -1678,9 +1681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14302A7-C5E8-40FF-86F2-64C01806B27A}">
   <dimension ref="A2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,10 +1729,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>7</v>
@@ -1750,13 +1753,13 @@
         <v>12</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>13</v>
@@ -1822,7 +1825,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
@@ -1835,7 +1838,9 @@
       <c r="J5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -1952,7 +1957,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2033,7 +2038,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2043,13 +2048,13 @@
         <v>3</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
@@ -2082,13 +2087,13 @@
         <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
@@ -2105,7 +2110,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2116,7 +2121,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>43</v>
@@ -2130,10 +2135,10 @@
         <v>44</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
@@ -2157,14 +2162,14 @@
         <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="7">
         <v>4</v>
@@ -2173,7 +2178,7 @@
         <v>41</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
@@ -2202,10 +2207,10 @@
         <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="7"/>
@@ -2213,10 +2218,10 @@
         <v>4</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>19</v>
@@ -2237,7 +2242,7 @@
         <v>365</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -2251,10 +2256,10 @@
         <v>42</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="7"/>
@@ -2262,10 +2267,10 @@
         <v>4</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>19</v>
@@ -2292,16 +2297,16 @@
         <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>18</v>
@@ -2321,7 +2326,7 @@
         <v>3000</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -2332,7 +2337,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -2343,7 +2348,7 @@
         <v>41</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>19</v>
@@ -2369,7 +2374,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -2377,10 +2382,10 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>35</v>
@@ -2404,13 +2409,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
@@ -2421,10 +2426,10 @@
         <v>27</v>
       </c>
       <c r="J19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="L19" s="23"/>
       <c r="M19" s="23"/>
@@ -2445,13 +2450,13 @@
         <v>15</v>
       </c>
       <c r="C20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="7"/>
@@ -2459,13 +2464,13 @@
         <v>5</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L20" s="23"/>
       <c r="M20" s="23"/>
@@ -2488,13 +2493,13 @@
         <v>15</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E21" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="7"/>
@@ -2502,13 +2507,13 @@
         <v>5</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L21" s="23"/>
       <c r="M21" s="23"/>
@@ -2531,29 +2536,29 @@
         <v>15</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L22" s="23"/>
       <c r="M22" s="23"/>
@@ -2576,29 +2581,29 @@
         <v>15</v>
       </c>
       <c r="C23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E23" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
         <v>6</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>18</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L23" s="23"/>
       <c r="M23" s="23"/>
@@ -2621,10 +2626,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -2634,10 +2639,10 @@
         <v>16</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L24" s="23"/>
       <c r="M24" s="23"/>
@@ -2663,7 +2668,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -2675,10 +2680,10 @@
         <v>16</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L25" s="23"/>
       <c r="M25" s="23"/>
@@ -2704,7 +2709,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -2719,7 +2724,7 @@
         <v>31</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
@@ -2742,7 +2747,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -2756,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
@@ -2796,22 +2801,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>93</v>
       </c>
       <c r="D2" s="25"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -2830,7 +2835,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -2846,32 +2851,32 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" t="s">
         <v>125</v>
-      </c>
-      <c r="G8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -2882,13 +2887,13 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -2896,47 +2901,47 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C25" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C26" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C27" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
@@ -2946,12 +2951,12 @@
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C35" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
@@ -2959,22 +2964,22 @@
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C40" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
@@ -2982,17 +2987,17 @@
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C47" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
@@ -3000,27 +3005,27 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C49" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C50" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C57" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
@@ -3028,17 +3033,17 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C59" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C61" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
@@ -3046,17 +3051,17 @@
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C68" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
@@ -3064,12 +3069,12 @@
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
@@ -3077,12 +3082,12 @@
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working with total energies and lcoe per iteration
</commit_message>
<xml_diff>
--- a/data/LCOE_Parameters.xlsx
+++ b/data/LCOE_Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f40ad5fc536dd58c/Desktop/Oxford/OPV/OPVSBSP_Code/OPV_SBSP/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanko\Desktop\personal\coding\OPV_SBSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6DF71121-27C4-4916-ACD1-3132EF372AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB17DDD8-8CA9-48E7-A0A1-D9B3E53CDC43}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D4D93-B7EF-4244-B4E6-F1AD5F4B2901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
   </bookViews>
@@ -870,9 +870,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -881,6 +878,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1681,9 +1681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14302A7-C5E8-40FF-86F2-64C01806B27A}">
   <dimension ref="A2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R19" sqref="B4:S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,7 +1802,7 @@
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
       <c r="O4" s="21"/>
-      <c r="P4" s="24">
+      <c r="P4" s="23">
         <v>0.03</v>
       </c>
       <c r="Q4" s="21"/>
@@ -1844,11 +1844,11 @@
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
-      <c r="O5" s="25">
+      <c r="O5" s="24">
         <v>100000</v>
       </c>
       <c r="P5" s="21"/>
-      <c r="Q5" s="25">
+      <c r="Q5" s="24">
         <v>2</v>
       </c>
       <c r="R5" s="21"/>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
-      <c r="N6" s="24">
+      <c r="N6" s="23">
         <v>0.15</v>
       </c>
       <c r="O6" s="21"/>
@@ -1936,11 +1936,11 @@
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="24">
+      <c r="O7" s="23">
         <v>4440000</v>
       </c>
       <c r="P7" s="21"/>
-      <c r="Q7" s="24">
+      <c r="Q7" s="23">
         <v>20.25</v>
       </c>
       <c r="R7" s="21"/>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
-      <c r="N9" s="25">
+      <c r="N9" s="24">
         <v>0.15</v>
       </c>
       <c r="O9" s="21"/>
@@ -2060,13 +2060,13 @@
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
-      <c r="N10" s="24">
+      <c r="N10" s="23">
         <v>0.1</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="24">
+      <c r="R10" s="23">
         <v>590</v>
       </c>
       <c r="S10" s="7" t="s">
@@ -2103,13 +2103,13 @@
       </c>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
-      <c r="N11" s="26">
+      <c r="N11" s="25">
         <v>10</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="26">
+      <c r="R11" s="25">
         <v>100</v>
       </c>
       <c r="S11" s="7"/>
@@ -2142,13 +2142,13 @@
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
-      <c r="N12" s="25">
+      <c r="N12" s="24">
         <v>0.08</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
-      <c r="R12" s="25">
+      <c r="R12" s="24">
         <v>1250</v>
       </c>
       <c r="S12" s="7"/>
@@ -2181,13 +2181,13 @@
       </c>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
-      <c r="N13" s="25">
+      <c r="N13" s="24">
         <v>0.3</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
-      <c r="R13" s="25">
+      <c r="R13" s="24">
         <v>150</v>
       </c>
       <c r="S13" s="7" t="s">
@@ -2269,7 +2269,9 @@
       <c r="O15" s="21"/>
       <c r="P15" s="21"/>
       <c r="Q15" s="21"/>
-      <c r="R15" s="15"/>
+      <c r="R15" s="15">
+        <v>0.4</v>
+      </c>
       <c r="S15" s="7"/>
     </row>
     <row r="16" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2388,19 +2390,19 @@
       <c r="K18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="23">
         <v>365</v>
       </c>
-      <c r="M18" s="24">
+      <c r="M18" s="23">
         <v>366</v>
       </c>
-      <c r="N18" s="24">
+      <c r="N18" s="23">
         <v>0.24249999999999999</v>
       </c>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
-      <c r="R18" s="24">
+      <c r="R18" s="23">
         <v>365</v>
       </c>
       <c r="S18" s="7" t="s">
@@ -2443,7 +2445,7 @@
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
-      <c r="R19" s="24">
+      <c r="R19" s="23">
         <v>24</v>
       </c>
       <c r="S19" s="7"/>
@@ -2472,17 +2474,17 @@
       <c r="K20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="24">
+      <c r="L20" s="23">
         <v>0.06</v>
       </c>
-      <c r="M20" s="24">
+      <c r="M20" s="23">
         <v>0.08</v>
       </c>
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="26">
+      <c r="R20" s="25">
         <v>0.4</v>
       </c>
       <c r="S20" s="7"/>
@@ -2517,7 +2519,7 @@
       <c r="O21" s="21"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="24">
+      <c r="R21" s="23">
         <v>20</v>
       </c>
       <c r="S21" s="7"/>
@@ -2558,7 +2560,7 @@
       <c r="O22" s="21"/>
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="26">
+      <c r="R22" s="25">
         <v>1000</v>
       </c>
       <c r="S22" s="7"/>
@@ -2595,13 +2597,13 @@
       </c>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
-      <c r="N23" s="26">
+      <c r="N23" s="25">
         <v>10</v>
       </c>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
-      <c r="R23" s="26">
+      <c r="R23" s="25">
         <v>100</v>
       </c>
       <c r="S23" s="7"/>
@@ -2638,13 +2640,13 @@
       </c>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
-      <c r="N24" s="26">
+      <c r="N24" s="25">
         <v>10</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
-      <c r="R24" s="26">
+      <c r="R24" s="25">
         <v>100</v>
       </c>
       <c r="S24" s="7"/>
@@ -2679,7 +2681,7 @@
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
-      <c r="N25" s="24">
+      <c r="N25" s="23">
         <v>0.15</v>
       </c>
       <c r="O25" s="21"/>
@@ -2721,11 +2723,11 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="24">
+      <c r="O26" s="23">
         <v>4440000</v>
       </c>
       <c r="P26" s="21"/>
-      <c r="Q26" s="24">
+      <c r="Q26" s="23">
         <v>20.25</v>
       </c>
       <c r="R26" s="21"/>
@@ -2795,10 +2797,10 @@
       <c r="B2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
changed parameters and it now follows the LCOE formula, needs checking
</commit_message>
<xml_diff>
--- a/data/LCOE_Parameters.xlsx
+++ b/data/LCOE_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanko\Desktop\personal\coding\OPV_SBSP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f40ad5fc536dd58c/Desktop/Oxford/OPV/OPVSBSP_Code/OPV_SBSP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF71121-27C4-4916-ACD1-3132EF372AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6DF71121-27C4-4916-ACD1-3132EF372AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB17DDD8-8CA9-48E7-A0A1-D9B3E53CDC43}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="128">
   <si>
     <t>LCOE</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Quaternary</t>
   </si>
   <si>
-    <t>Quintenary</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -102,15 +99,9 @@
     <t>Repairs</t>
   </si>
   <si>
-    <t>Material Repairs</t>
-  </si>
-  <si>
     <t>Exponential</t>
   </si>
   <si>
-    <t>Yearly (random?)</t>
-  </si>
-  <si>
     <t>Assumes costs will increase sharply with unexpected failures.</t>
   </si>
   <si>
@@ -150,12 +141,6 @@
     <t>Fuel cost</t>
   </si>
   <si>
-    <t>£/m3</t>
-  </si>
-  <si>
-    <t>Marketprice with fluctuations - Include sensitivity?</t>
-  </si>
-  <si>
     <t>Emission Cost</t>
   </si>
   <si>
@@ -177,27 +162,12 @@
     <t>Y0</t>
   </si>
   <si>
-    <t>Efficiency (n)</t>
-  </si>
-  <si>
-    <t>#days in year x</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
     <t>Depends on year to account for leap years</t>
   </si>
   <si>
-    <t>MWh</t>
-  </si>
-  <si>
     <t>Log-normal</t>
   </si>
   <si>
-    <t>Planned corrections per year</t>
-  </si>
-  <si>
     <t>Depreciation of Assets</t>
   </si>
   <si>
@@ -216,36 +186,12 @@
     <t xml:space="preserve">Manufacture Panels </t>
   </si>
   <si>
-    <t>Number of panels</t>
-  </si>
-  <si>
     <t>Raw Materials</t>
   </si>
   <si>
     <t>Processing</t>
   </si>
   <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>Distance of transport</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>Cost of Fuel</t>
-  </si>
-  <si>
-    <t>£/km</t>
-  </si>
-  <si>
-    <t>Deployment</t>
-  </si>
-  <si>
-    <t>Logistics Costs</t>
-  </si>
-  <si>
     <t>Number of Launches</t>
   </si>
   <si>
@@ -270,22 +216,10 @@
     <t>Total emissions</t>
   </si>
   <si>
-    <t>CO2e/MWh</t>
-  </si>
-  <si>
-    <t>£/CO2e</t>
-  </si>
-  <si>
     <t>n(year) = n(Y0) + -degradation(n) + repairs(n)</t>
   </si>
   <si>
     <t>Hours in a day</t>
-  </si>
-  <si>
-    <t>Energy consumption</t>
-  </si>
-  <si>
-    <t>Total Energy =( Installed capacity * n(for each year)* days in a year *hours in a day)  - Energy consumption</t>
   </si>
   <si>
     <t>Energy Genrated</t>
@@ -625,13 +559,70 @@
     <t>Bernoulli</t>
   </si>
   <si>
-    <t>£/panel</t>
-  </si>
-  <si>
     <t>Exact</t>
   </si>
   <si>
     <t>Yearly (to be in all arrays needed ;*)</t>
+  </si>
+  <si>
+    <t>Quinary</t>
+  </si>
+  <si>
+    <t>Probability of Material Repairs</t>
+  </si>
+  <si>
+    <t>Yearly (random)</t>
+  </si>
+  <si>
+    <t>Launch Repair</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Repair Assembly</t>
+  </si>
+  <si>
+    <t>USD/m3</t>
+  </si>
+  <si>
+    <t>Marketprice with fluctuations - Include sensitivity</t>
+  </si>
+  <si>
+    <t>Energy system emissions</t>
+  </si>
+  <si>
+    <t>tCO2e/m2</t>
+  </si>
+  <si>
+    <t>Launching emissions</t>
+  </si>
+  <si>
+    <t>tCO2e/launch</t>
+  </si>
+  <si>
+    <t>USD/tCO2e</t>
+  </si>
+  <si>
+    <t>Original Efficiency</t>
+  </si>
+  <si>
+    <t>Efficiency Degradation Rate</t>
+  </si>
+  <si>
+    <t>Efficiency boost repair</t>
+  </si>
+  <si>
+    <t>#days in year t</t>
+  </si>
+  <si>
+    <t>Area of panels</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>£/m2</t>
   </si>
 </sst>
 </file>
@@ -663,7 +654,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,18 +735,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -763,6 +742,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -807,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -854,12 +851,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -873,14 +864,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1336,27 +1336,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{909B92F7-FD86-4123-9D2B-E5C0FFDF9F53}" name="Table142" displayName="Table142" ref="B3:S27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
-  <autoFilter ref="B3:S27" xr:uid="{909B92F7-FD86-4123-9D2B-E5C0FFDF9F53}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B08AEF9E-068D-41A3-8F97-8D12F6EF653C}" name="Table1423" displayName="Table1423" ref="B3:S27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="B3:S27" xr:uid="{B08AEF9E-068D-41A3-8F97-8D12F6EF653C}"/>
   <tableColumns count="18">
-    <tableColumn id="2" xr3:uid="{AE1E91F8-E08D-4870-9EA0-9D766B95EB09}" name="Primary" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{117D9C5B-B5EB-4229-8E6B-F43AA68FDD63}" name="Secondary" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{E20BFF9A-E6DB-4DA8-B61C-78AD62869AB0}" name="Tertiary" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{AC0B1E94-75E6-4D82-93A4-33F5480F0B94}" name="Quaternary" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{C1AC552C-A369-4000-876A-E0CEC4E0E60C}" name="Quintenary" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{DCB5AB7C-8BE9-4156-8808-C7844619DC70}" name="Relationships" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{E494D826-7428-44F0-8A41-82212B791038}" name="Multiplied" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{9562A130-14D3-4A9B-9FC6-6563E1EBD9FD}" name="Units" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{0E83D34C-CD9E-4572-948B-530B8A0AC574}" name="Distribution" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{F85CB51D-AECB-435B-8E6E-86A6A19C6EE6}" name="Time for determination (Year)" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{796FC7BB-E419-482C-AED0-2D0EC27F353E}" name="Lower Limit" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{E8F799E3-4165-4BB4-B4E3-E0AC59BF7E53}" name="Upper Limit" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A05EEDE8-7B8A-4237-951E-78D9F4E5CDCF}" name="SD" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{0CF3F9E6-935B-4AB5-8103-35660404BC57}" name="Scale" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{ED5B0C21-BE1E-4570-BC5D-006BB2D1AC04}" name="Count" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{405E56AE-8602-44F1-B0E5-88A5D58A6492}" name="Shape" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{BD72848E-BEE6-471B-BAF7-23A9FDE1B8A8}" name="Mean" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{3CF19983-7617-4E79-BA6C-E9BD88BF77AC}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{369F9D63-7381-41DE-AF54-F61FEF03A055}" name="Primary" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{A508656A-BBD0-4725-8C30-906CCEF7AD73}" name="Secondary" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{2AB616BE-FCF5-42D2-92ED-6984504DD689}" name="Tertiary" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{52434BF0-87B9-49A6-89B5-358411B16EE7}" name="Quaternary" dataDxfId="14"/>
+    <tableColumn id="16" xr3:uid="{F2F64508-351A-4118-923C-04DF33C4BB18}" name="Quinary" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{BC6144CE-7929-4A4E-9441-EDC50DFE6922}" name="Relationships" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{727A3DF3-5FC4-42D3-8FA1-FEF1EBCF53E0}" name="Multiplied" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{C284C7FD-5580-4E7D-B408-0161A8B5E19F}" name="Units" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FDBF8740-5BA9-460E-9F8E-6E27BAB10B27}" name="Distribution" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{93EBFF29-EC92-40F1-A935-56C91E979DAB}" name="Time for determination (Year)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2115A830-BC7B-46BB-80E4-AF757613117E}" name="Lower Limit" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{6AF9E6A2-703C-43D6-89CD-C843176FB3CA}" name="Upper Limit" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{189E40B7-959A-4450-8478-76C30236A444}" name="SD" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{F383F33D-34AD-4A2E-BEE4-D9F9654775BE}" name="Scale" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{DE47C2C3-F36C-4B07-8C94-518CD3244245}" name="Count" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{90EC11DF-0AD4-41B8-B230-D22EBA3CBA4D}" name="Shape" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{A66F4D24-CA10-453B-AAD5-FAD84E3D4A0F}" name="Mean" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{F68E6CE9-8247-436E-90ED-50F7BD7D258E}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1681,9 +1681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14302A7-C5E8-40FF-86F2-64C01806B27A}">
   <dimension ref="A2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,46 +1726,46 @@
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -1773,16 +1773,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="7"/>
@@ -1790,25 +1790,25 @@
         <v>18</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23">
-        <v>20</v>
-      </c>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
+        <v>110</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
       <c r="S4" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1816,16 +1816,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
@@ -1833,25 +1833,25 @@
         <v>18</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23">
-        <v>1000</v>
-      </c>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23">
+        <v>18</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="25">
+        <v>100000</v>
+      </c>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="25">
         <v>2</v>
       </c>
-      <c r="R5" s="23"/>
+      <c r="R5" s="21"/>
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1859,44 +1859,46 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7">
         <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23">
-        <v>0.03</v>
-      </c>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
+        <v>40</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="15">
+        <v>10</v>
+      </c>
       <c r="S6" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -1904,46 +1906,46 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7">
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23">
-        <v>1000</v>
-      </c>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23">
-        <v>2</v>
-      </c>
-      <c r="R7" s="23"/>
+        <v>110</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="24">
+        <v>4440000</v>
+      </c>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="24">
+        <v>20.25</v>
+      </c>
+      <c r="R7" s="21"/>
       <c r="S7" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1951,54 +1953,54 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7">
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22">
+        <v>10000</v>
+      </c>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22">
         <v>2</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23">
-        <v>5000</v>
-      </c>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23">
-        <v>50000</v>
-      </c>
-      <c r="S8" s="7"/>
-    </row>
-    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R8" s="22"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -2007,79 +2009,83 @@
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23">
-        <v>2</v>
-      </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23">
-        <v>10</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>38</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="15">
+        <v>50000</v>
+      </c>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23">
-        <v>10</v>
-      </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23">
-        <v>100</v>
-      </c>
-      <c r="S10" s="7"/>
-    </row>
-    <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="24">
+        <v>590</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="7"/>
@@ -2087,67 +2093,63 @@
         <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23">
-        <v>3</v>
-      </c>
-      <c r="S11" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="26">
+        <v>10</v>
+      </c>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="26">
+        <v>100</v>
+      </c>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>42</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7">
-        <v>4</v>
-      </c>
+      <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>129</v>
+        <v>17</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23">
-        <v>2000</v>
+        <v>40</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="25">
+        <v>1250</v>
       </c>
       <c r="S12" s="7"/>
     </row>
@@ -2156,61 +2158,57 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23">
-        <v>-0.69889999999999997</v>
-      </c>
-      <c r="S13" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="25">
+        <v>150</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="7"/>
@@ -2218,227 +2216,235 @@
         <v>4</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="23">
-        <v>365</v>
-      </c>
-      <c r="M14" s="23">
-        <v>366</v>
-      </c>
-      <c r="N14" s="23">
-        <v>0.24249999999999999</v>
-      </c>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23">
-        <v>365</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>49</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="15">
+        <v>2000</v>
+      </c>
+      <c r="S14" s="7"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="7">
-        <v>4</v>
-      </c>
+      <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23">
-        <v>24</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="15"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:19" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="H16" s="7">
+        <v>4</v>
+      </c>
       <c r="I16" s="7" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="J16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23">
-        <v>30</v>
-      </c>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23">
-        <v>3000</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="15">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="S16" s="7"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="23">
-        <v>0.06</v>
-      </c>
-      <c r="M17" s="23">
-        <v>0.08</v>
-      </c>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
+        <v>18</v>
+      </c>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="15">
+        <v>0.05</v>
+      </c>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7">
+        <v>4</v>
+      </c>
       <c r="I18" s="7" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23">
-        <v>20</v>
-      </c>
-      <c r="S18" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="L18" s="24">
+        <v>365</v>
+      </c>
+      <c r="M18" s="24">
+        <v>366</v>
+      </c>
+      <c r="N18" s="24">
+        <v>0.24249999999999999</v>
+      </c>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="24">
+        <v>365</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>58</v>
+        <v>14</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23">
-        <v>1000</v>
+        <v>18</v>
+      </c>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="24">
+        <v>24</v>
       </c>
       <c r="S19" s="7"/>
     </row>
@@ -2447,41 +2453,37 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="7">
-        <v>5</v>
-      </c>
+      <c r="H20" s="7"/>
       <c r="I20" s="7" t="s">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="J20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23">
-        <v>10</v>
-      </c>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23">
-        <v>100</v>
+      <c r="L20" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="M20" s="24">
+        <v>0.08</v>
+      </c>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="26">
+        <v>0.4</v>
       </c>
       <c r="S20" s="7"/>
     </row>
@@ -2490,41 +2492,33 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>61</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="7">
-        <v>5</v>
-      </c>
+      <c r="H21" s="7"/>
       <c r="I21" s="7" t="s">
-        <v>128</v>
+        <v>46</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23">
-        <v>10</v>
-      </c>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23">
-        <v>100</v>
+        <v>32</v>
+      </c>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="24">
+        <v>20</v>
       </c>
       <c r="S21" s="7"/>
     </row>
@@ -2533,43 +2527,39 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>63</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="5"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23">
-        <v>10</v>
-      </c>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23">
-        <v>200</v>
+        <v>40</v>
+      </c>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="26">
+        <v>1000</v>
       </c>
       <c r="S22" s="7"/>
     </row>
@@ -2578,43 +2568,41 @@
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="5"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23">
-        <v>2</v>
-      </c>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23">
-        <v>20</v>
+        <v>40</v>
+      </c>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="26">
+        <v>10</v>
+      </c>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="26">
+        <v>100</v>
       </c>
       <c r="S23" s="7"/>
     </row>
@@ -2623,37 +2611,41 @@
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="H24" s="7">
+        <v>5</v>
+      </c>
       <c r="I24" s="7" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23">
-        <v>20</v>
-      </c>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23">
-        <v>200</v>
+        <v>40</v>
+      </c>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="26">
+        <v>10</v>
+      </c>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="26">
+        <v>100</v>
       </c>
       <c r="S24" s="7"/>
     </row>
@@ -2662,13 +2654,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -2677,23 +2669,23 @@
         <v>7</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23">
-        <v>20</v>
-      </c>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23">
+        <v>40</v>
+      </c>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="15">
         <v>200</v>
       </c>
       <c r="S25" s="7"/>
@@ -2703,13 +2695,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -2718,25 +2710,25 @@
         <v>7</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23">
-        <v>1000</v>
-      </c>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23">
-        <v>2</v>
-      </c>
-      <c r="R26" s="23"/>
+        <v>40</v>
+      </c>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="24">
+        <v>4440000</v>
+      </c>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="24">
+        <v>20.25</v>
+      </c>
+      <c r="R26" s="21"/>
       <c r="S26" s="7"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2744,37 +2736,37 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24">
-        <v>1000</v>
-      </c>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24">
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22">
+        <v>100000</v>
+      </c>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22">
         <v>2</v>
       </c>
-      <c r="R27" s="24"/>
-      <c r="S27" s="18"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2801,293 +2793,293 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="25"/>
+        <v>69</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
-        <v>27</v>
+      <c r="B15" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
-        <v>95</v>
+      <c r="B16" s="17" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
-        <v>96</v>
+      <c r="B17" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
-        <v>97</v>
+      <c r="B18" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
-        <v>98</v>
+      <c r="B19" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C25" s="19" t="s">
-        <v>100</v>
+      <c r="C25" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C26" s="19" t="s">
-        <v>101</v>
+      <c r="C26" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="19" t="s">
-        <v>102</v>
+      <c r="C27" s="17" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C35" s="20" t="s">
-        <v>104</v>
+      <c r="C35" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="21"/>
+      <c r="C36" s="19"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="22" t="s">
-        <v>105</v>
+      <c r="C37" s="20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="22" t="s">
-        <v>106</v>
+      <c r="C38" s="20" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C40" s="20" t="s">
-        <v>107</v>
+      <c r="C40" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="21"/>
+      <c r="C43" s="19"/>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="21" t="s">
-        <v>109</v>
+      <c r="C44" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="21" t="s">
-        <v>110</v>
+      <c r="C45" s="19" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C47" s="20" t="s">
-        <v>111</v>
+      <c r="C47" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="21"/>
+      <c r="C48" s="19"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="22" t="s">
-        <v>112</v>
+      <c r="C49" s="20" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="22" t="s">
-        <v>113</v>
+      <c r="C50" s="20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C57" s="20" t="s">
-        <v>104</v>
+      <c r="C57" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C58" s="21"/>
+      <c r="C58" s="19"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C59" s="22" t="s">
-        <v>115</v>
+      <c r="C59" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C61" s="20" t="s">
-        <v>107</v>
+      <c r="C61" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C64" s="21"/>
+      <c r="C64" s="19"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C65" s="21" t="s">
-        <v>117</v>
+      <c r="C65" s="19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="21" t="s">
-        <v>118</v>
+      <c r="C66" s="19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C68" s="20" t="s">
-        <v>119</v>
+      <c r="C68" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C69" s="21"/>
+      <c r="C69" s="19"/>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C70" s="22" t="s">
-        <v>120</v>
+      <c r="C70" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C73" s="21"/>
+      <c r="C73" s="19"/>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C74" s="21" t="s">
-        <v>122</v>
+      <c r="C74" s="19" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C75" s="21" t="s">
-        <v>123</v>
+      <c r="C75" s="19" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>